<commit_message>
RESTful WS with Jersey
RESTful WS with Jersey
</commit_message>
<xml_diff>
--- a/Requirements/requirements.xlsx
+++ b/Requirements/requirements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Bug Description and reproduce steps</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>On clicking attachment icon in definitions table -&gt; open another tab/model window -&gt; display images are album</t>
+  </si>
+  <si>
+    <t>Implement ng-table for Definitions table</t>
   </si>
 </sst>
 </file>
@@ -408,11 +411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -450,6 +453,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +469,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -490,6 +498,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>